<commit_message>
- NhapKhoNoiBo: add some column {Ma,TenNCC}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_PhieuNhapKhoNoiBo.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_PhieuNhapKhoNoiBo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tổng tiền hàng</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t>DANH SÁCH TỔNG HỢP PHIẾU NHẬP KHO NỘI BỘ</t>
+  </si>
+  <si>
+    <t>Mã nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Tên nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Phải thanh toán</t>
+  </si>
+  <si>
+    <t>Đã thanh toán</t>
+  </si>
+  <si>
+    <t>Còn nợ</t>
   </si>
 </sst>
 </file>
@@ -152,7 +167,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -203,29 +218,38 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -537,294 +561,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="22.42578125" style="23" customWidth="1"/>
+    <col min="3" max="4" width="22.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="16" customWidth="1"/>
+    <col min="7" max="9" width="23.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" style="16" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:12" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="17">
-        <f>SUM(E5:E28)</f>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="17">
+        <f t="shared" ref="G29:I29" si="0">SUM(G5:G28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="H29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <f>SUM(J5:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>